<commit_message>
week 4 scores again
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_49.xlsx
+++ b/data/PointsScored_Survivor_49.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFBD4F2-FB4B-4707-AEE1-B450868B0189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F923F4-173A-45A7-8247-25B6BAF66E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="PointsScored_Survivor" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="83">
   <si>
     <t>Player</t>
   </si>
@@ -258,17 +258,57 @@
   </si>
   <si>
     <t>Exits due to health/injury before merge</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Who will say the episode title "Go Kick Rocks, Bro"?</t>
+  </si>
+  <si>
+    <t>Who will find an advantage/idol etc.?</t>
+  </si>
+  <si>
+    <t>Who will be on the winning immunity challenge team? (pick one person, tribe swap time!)</t>
+  </si>
+  <si>
+    <t>Who will be on the winning reward challenge team?</t>
+  </si>
+  <si>
+    <t>Will anyone play a shot in the dark?</t>
+  </si>
+  <si>
+    <t>Will anyone play an idol/advantage at tribal?</t>
+  </si>
+  <si>
+    <t>Will anyone cry?</t>
+  </si>
+  <si>
+    <t>Who will be eliminated?</t>
+  </si>
+  <si>
+    <t>Shannon, Alex, Steven, Sage, MC, Kristina, Sophie S</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,12 +367,24 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -360,18 +412,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,11 +650,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1357,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E990"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1435,10 +1496,21 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>4</v>
+      </c>
+      <c r="E5" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -2474,10 +2546,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABC1FEC-B626-46F0-AE97-C498D904E4E1}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2596,7 @@
       <c r="B2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E2">
@@ -2547,7 +2619,7 @@
       <c r="B3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E3">
@@ -2570,7 +2642,7 @@
       <c r="B4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="13" t="s">
         <v>69</v>
       </c>
       <c r="E4">
@@ -2584,6 +2656,214 @@
       </c>
       <c r="H4">
         <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
week 4 scores again again
</commit_message>
<xml_diff>
--- a/data/PointsScored_Survivor_49.xlsx
+++ b/data/PointsScored_Survivor_49.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F923F4-173A-45A7-8247-25B6BAF66E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF46125-F092-48C3-A7F0-E30213FCD1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A549BF43-C147-4A07-BF22-B3F340E87A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="PointsScored_Survivor" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -424,7 +424,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -650,11 +649,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C68" sqref="C68"/>
+      <selection pane="bottomRight" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1418,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E990"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2596,7 +2595,7 @@
       <c r="B2" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E2">
@@ -2619,7 +2618,7 @@
       <c r="B3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E3">
@@ -2642,7 +2641,7 @@
       <c r="B4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>69</v>
       </c>
       <c r="E4">
@@ -2662,13 +2661,13 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E5" t="s">
@@ -2688,13 +2687,13 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>72</v>
       </c>
       <c r="E6" t="s">
@@ -2714,22 +2713,22 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>58</v>
       </c>
       <c r="F7" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>57</v>
       </c>
       <c r="H7" t="s">
@@ -2743,22 +2742,22 @@
       <c r="B8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2769,22 +2768,22 @@
       <c r="B9" t="s">
         <v>77</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>72</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2795,22 +2794,22 @@
       <c r="B10" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="11" t="s">
         <v>72</v>
       </c>
       <c r="F10" t="s">
         <v>69</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2818,22 +2817,22 @@
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>69</v>
       </c>
       <c r="H11" t="s">
@@ -2844,16 +2843,16 @@
       <c r="A12">
         <v>4</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>57</v>
       </c>
       <c r="F12" t="s">

</xml_diff>